<commit_message>
naming conventions updated in excel
</commit_message>
<xml_diff>
--- a/CapstonePlan.xlsx
+++ b/CapstonePlan.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devanandh.v\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF57C07-A313-423A-A4E1-15BC4AA22C55}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D644960-E149-4939-9C70-6B2DDF5B8177}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="110">
   <si>
     <t>Milestone 1</t>
   </si>
@@ -303,6 +303,109 @@
   </si>
   <si>
     <t>Prabhakaran/Devanandh/Karan</t>
+  </si>
+  <si>
+    <t>house_df_out3</t>
+  </si>
+  <si>
+    <t>X_base</t>
+  </si>
+  <si>
+    <t>y_base</t>
+  </si>
+  <si>
+    <t>Dataframe name</t>
+  </si>
+  <si>
+    <t>X_name</t>
+  </si>
+  <si>
+    <t>y_name</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>train_base</t>
+  </si>
+  <si>
+    <t>test_base</t>
+  </si>
+  <si>
+    <t>train_labels_base</t>
+  </si>
+  <si>
+    <t>Train_labels</t>
+  </si>
+  <si>
+    <t>Test_labels</t>
+  </si>
+  <si>
+    <t>test_labels_base</t>
+  </si>
+  <si>
+    <t>house_df_base</t>
+  </si>
+  <si>
+    <t>house_df_new-&gt;</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>house_df_scaled_out1
+house_df_scaled_out2
+house_df_scaled_out3</t>
+  </si>
+  <si>
+    <t>X_scaled</t>
+  </si>
+  <si>
+    <t>y_scaled</t>
+  </si>
+  <si>
+    <t>train_scaled</t>
+  </si>
+  <si>
+    <t>test_scaled</t>
+  </si>
+  <si>
+    <t>train_labels_scaled</t>
+  </si>
+  <si>
+    <t>test_labels_scaled</t>
+  </si>
+  <si>
+    <t>house_df_out1-&gt;
+house_df_out_2-&gt;
+house_df_out3-&gt;</t>
+  </si>
+  <si>
+    <t>house_df_scaled3-&gt;</t>
+  </si>
+  <si>
+    <t>house_df_pca</t>
+  </si>
+  <si>
+    <t>X_pca</t>
+  </si>
+  <si>
+    <t>y_pca</t>
+  </si>
+  <si>
+    <t>train_pca</t>
+  </si>
+  <si>
+    <t>test_pca</t>
+  </si>
+  <si>
+    <t>train_labels_pca</t>
+  </si>
+  <si>
+    <t>test_labels_pca</t>
   </si>
 </sst>
 </file>
@@ -483,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -526,6 +629,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,9 +679,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:I39" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A2:I39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:J39" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A2:J39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Activity"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SubTask"/>
@@ -584,6 +691,7 @@
     <tableColumn id="7" xr3:uid="{9321816D-87D0-4473-86FE-92F687E9065E}" name="Column2"/>
     <tableColumn id="8" xr3:uid="{B4F51F0F-06DF-40B2-9D20-94E45B7869A1}" name="Column3"/>
     <tableColumn id="9" xr3:uid="{B29ED9D9-B72B-4ADB-A580-F637CBF2EEAD}" name="Column4"/>
+    <tableColumn id="10" xr3:uid="{F48B940A-455E-41E0-8C06-6DD0CEF6FAC0}" name="Column5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -852,10 +960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I39"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="F22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,16 +976,20 @@
     <col min="5" max="5" width="36.7109375" style="24" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -904,8 +1017,11 @@
       <c r="I2" s="21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -917,7 +1033,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
@@ -932,7 +1048,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -947,7 +1063,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
@@ -955,7 +1071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5"/>
@@ -963,7 +1079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="2"/>
       <c r="C8" s="5"/>
@@ -971,14 +1087,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="2"/>
       <c r="C10" s="5" t="s">
@@ -991,7 +1107,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
@@ -1001,7 +1117,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5" t="s">
@@ -1011,7 +1127,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5" t="s">
@@ -1021,7 +1137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5" t="s">
@@ -1034,7 +1150,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="2"/>
       <c r="C15" s="5"/>
@@ -1042,7 +1158,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1052,7 +1168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
@@ -1062,7 +1178,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="2"/>
       <c r="C18" s="18" t="s">
@@ -1075,7 +1191,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="2"/>
       <c r="C19" s="5" t="s">
@@ -1085,7 +1201,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="2"/>
       <c r="C20" s="5" t="s">
@@ -1095,7 +1211,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="2"/>
       <c r="C21" s="18" t="s">
@@ -1105,7 +1221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="8"/>
       <c r="C22" s="19" t="s">
@@ -1114,8 +1230,29 @@
       <c r="D22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="K22" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q22" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>1</v>
       </c>
@@ -1132,8 +1269,11 @@
       <c r="H23" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>10</v>
       </c>
@@ -1153,8 +1293,32 @@
       <c r="H24" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" t="s">
+        <v>91</v>
+      </c>
+      <c r="L24" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" t="s">
+        <v>79</v>
+      </c>
+      <c r="N24" t="s">
+        <v>85</v>
+      </c>
+      <c r="O24" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>11</v>
       </c>
@@ -1177,8 +1341,32 @@
       <c r="I25" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J25" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" t="s">
+        <v>95</v>
+      </c>
+      <c r="M25" t="s">
+        <v>96</v>
+      </c>
+      <c r="N25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" t="s">
+        <v>98</v>
+      </c>
+      <c r="P25" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="2"/>
       <c r="C26" s="5" t="s">
@@ -1199,8 +1387,32 @@
       <c r="I26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>102</v>
+      </c>
+      <c r="K26" t="s">
+        <v>103</v>
+      </c>
+      <c r="L26" t="s">
+        <v>104</v>
+      </c>
+      <c r="M26" t="s">
+        <v>105</v>
+      </c>
+      <c r="N26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P26" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="2"/>
       <c r="C27" s="5"/>
@@ -1214,7 +1426,7 @@
         <v>43539</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="2"/>
       <c r="C28" s="5"/>
@@ -1231,7 +1443,7 @@
         <v>43540</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="2"/>
       <c r="C29" s="5"/>
@@ -1248,7 +1460,7 @@
         <v>43540</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -1267,14 +1479,14 @@
         <v>43540</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="2"/>
       <c r="C31" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="2"/>
       <c r="C32" s="5" t="s">

</xml_diff>